<commit_message>
Initial commit for  version 2
</commit_message>
<xml_diff>
--- a/firmware/pins.xlsx
+++ b/firmware/pins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirillov\Dropbox\Robotics\github\motor-driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirillov\Dropbox\Robotics\github\motor-driver\firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,42 +50,6 @@
     <t>NEOPIXEL</t>
   </si>
   <si>
-    <t>D0</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D12</t>
-  </si>
-  <si>
-    <t>D13</t>
-  </si>
-  <si>
-    <t>D14</t>
-  </si>
-  <si>
-    <t>D15</t>
-  </si>
-  <si>
-    <t>D16</t>
-  </si>
-  <si>
-    <t>D17</t>
-  </si>
-  <si>
     <t>Motor driver pin assignments</t>
   </si>
   <si>
@@ -95,12 +59,6 @@
     <t>M2_PWM</t>
   </si>
   <si>
-    <t>JMP2</t>
-  </si>
-  <si>
-    <t>JMP1</t>
-  </si>
-  <si>
     <t>ENC2_B</t>
   </si>
   <si>
@@ -119,68 +77,110 @@
     <t>M1_PWM</t>
   </si>
   <si>
-    <t>D18</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>Not broken out</t>
-  </si>
-  <si>
     <t>I2C</t>
   </si>
   <si>
-    <t>PWM1B</t>
-  </si>
-  <si>
     <t>PIO0</t>
   </si>
   <si>
-    <t>A0=D26</t>
-  </si>
-  <si>
-    <t>A1=D27</t>
-  </si>
-  <si>
-    <t>A2=D28</t>
-  </si>
-  <si>
     <t>PWM6A</t>
   </si>
   <si>
     <t>PIO1</t>
   </si>
   <si>
-    <t>I2C address bit 0</t>
-  </si>
-  <si>
-    <t>I2C address bit 1</t>
-  </si>
-  <si>
     <t>Error status flag for driver1</t>
   </si>
   <si>
     <t>Error status flag for driver2</t>
   </si>
   <si>
-    <t>DISABLE</t>
-  </si>
-  <si>
-    <t>Disables both motor drivers</t>
-  </si>
-  <si>
-    <t>M2_ERROR</t>
-  </si>
-  <si>
-    <t>M1_ERROR</t>
+    <t>GPIO0</t>
+  </si>
+  <si>
+    <t>GPIO1</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>GPIO3</t>
+  </si>
+  <si>
+    <t>GPIO5</t>
+  </si>
+  <si>
+    <t>M2_FLAG</t>
+  </si>
+  <si>
+    <t>GPIO10</t>
+  </si>
+  <si>
+    <t>GPIO6</t>
+  </si>
+  <si>
+    <t>GPIO7</t>
+  </si>
+  <si>
+    <t>GPIO11</t>
+  </si>
+  <si>
+    <t>M2_ENABLE</t>
+  </si>
+  <si>
+    <t>GPIO12</t>
+  </si>
+  <si>
+    <t>GPIO13</t>
+  </si>
+  <si>
+    <t>GPIO14</t>
+  </si>
+  <si>
+    <t>GPIO18</t>
+  </si>
+  <si>
+    <t>GPIO19</t>
+  </si>
+  <si>
+    <t>ADDR_0</t>
+  </si>
+  <si>
+    <t>ADDR_1</t>
+  </si>
+  <si>
+    <t>ADDR_2</t>
+  </si>
+  <si>
+    <t>GPIO20</t>
+  </si>
+  <si>
+    <t>GPIO24</t>
+  </si>
+  <si>
+    <t>M1_FLAG</t>
+  </si>
+  <si>
+    <t>GPIO27</t>
+  </si>
+  <si>
+    <t>M1_ENABLE</t>
+  </si>
+  <si>
+    <t>GPIO28</t>
+  </si>
+  <si>
+    <t>PWM5A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,14 +196,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,12 +207,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -269,8 +257,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,10 +580,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,12 +595,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -627,15 +613,15 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
@@ -644,10 +630,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
@@ -656,169 +642,181 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="A15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>